<commit_message>
modified:   assets/form/TOAZD.xlsx 	modified:   lib/model_udz.dart 	modified:   lib/object_detail_azd.dart 	modified:   lib/object_detail_ukz.dart 	modified:   lib/object_detail_upz.dart 	modified:   lib/object_list_azd.dart 	modified:   pubspec.yaml
</commit_message>
<xml_diff>
--- a/assets/form/TOAZD.xlsx
+++ b/assets/form/TOAZD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\flutterDartProjects\ehz1\assets\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AADAE299-5519-4769-9734-72235998A600}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905DCDAC-862D-4369-97EB-2E165BE23F0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21F93581-3072-4921-A15F-763FA22ADC48}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21F93581-3072-4921-A15F-763FA22ADC48}"/>
   </bookViews>
   <sheets>
     <sheet name="TOAZD" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">TOAZD!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Тип контроля</t>
   </si>
@@ -56,105 +55,6 @@
   </si>
   <si>
     <t>Удельное сопротивление грунта, Ом*м</t>
-  </si>
-  <si>
-    <t> int</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>todoDate</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>kontrol</t>
-  </si>
-  <si>
-    <t>kolvoprotvgruppe</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>fotoupz</t>
-  </si>
-  <si>
-    <t>zamechupz</t>
-  </si>
-  <si>
-    <t>sostojanieupz</t>
-  </si>
-  <si>
-    <t>potencialvklpolyar</t>
-  </si>
-  <si>
-    <t>potencialprot</t>
-  </si>
-  <si>
-    <t>edsupz</t>
-  </si>
-  <si>
-    <t>tokupz</t>
-  </si>
-  <si>
-    <t>soprrast</t>
-  </si>
-  <si>
-    <t>udsoprgrunta</t>
-  </si>
-  <si>
-    <t>potencialvklsumm1</t>
-  </si>
-  <si>
-    <t>potencialvklpolyar1</t>
-  </si>
-  <si>
-    <t>potencialprot1</t>
-  </si>
-  <si>
-    <t>edsupz1</t>
-  </si>
-  <si>
-    <t>tokupz1</t>
-  </si>
-  <si>
-    <t>soprrast1</t>
-  </si>
-  <si>
-    <t>udsoprgrunta1</t>
-  </si>
-  <si>
-    <t>potencialvklsumm2</t>
-  </si>
-  <si>
-    <t>potencialvklpolyar2</t>
-  </si>
-  <si>
-    <t>potencialprot2</t>
-  </si>
-  <si>
-    <t>edsupz2</t>
-  </si>
-  <si>
-    <t>tokupz2</t>
-  </si>
-  <si>
-    <t>soprrast2</t>
-  </si>
-  <si>
-    <t>udsoprgrunta2</t>
-  </si>
-  <si>
-    <t>Протокол обслуживания перехода через АЖД №</t>
   </si>
   <si>
     <t>До перехода по ходу газа</t>
@@ -781,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71296316-4C04-4862-968C-7E51A3A0E192}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,9 +700,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>39</v>
-      </c>
+      <c r="A1" s="23"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -829,256 +727,136 @@
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="6" t="str">
-        <f>"this."&amp;J3&amp;","</f>
-        <v>this.id,</v>
-      </c>
-      <c r="N3" s="6" t="str">
-        <f>"String get "&amp;J3&amp;" =&gt; _"&amp;J3&amp;";"</f>
-        <v>String get id =&gt; _id;</v>
-      </c>
+      <c r="H3" s="16"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="18" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="18" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="6" t="str">
-        <f t="shared" ref="L4:L37" si="0">"this."&amp;J4&amp;","</f>
-        <v>this.todoDate,</v>
-      </c>
-      <c r="N4" s="6" t="str">
-        <f t="shared" ref="N4:N37" si="1">"String get "&amp;J4&amp;" =&gt; _"&amp;J4&amp;";"</f>
-        <v>String get todoDate =&gt; _todoDate;</v>
-      </c>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="18" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="18" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.title,</v>
-      </c>
-      <c r="N5" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get title =&gt; _title;</v>
-      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="18" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="18" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.kontrol,</v>
-      </c>
-      <c r="N6" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get kontrol =&gt; _kontrol;</v>
-      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.kolvoprotvgruppe,</v>
-      </c>
-      <c r="N7" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get kolvoprotvgruppe =&gt; _kolvoprotvgruppe;</v>
-      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="18" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="18" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.date,</v>
-      </c>
-      <c r="N8" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get date =&gt; _date;</v>
-      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="18" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="18" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.fotoupz,</v>
-      </c>
-      <c r="N9" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get fotoupz =&gt; _fotoupz;</v>
-      </c>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="18" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="18" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.zamechupz,</v>
-      </c>
-      <c r="N10" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get zamechupz =&gt; _zamechupz;</v>
-      </c>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
@@ -1086,43 +864,27 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="18" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="18" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.sostojanieupz,</v>
-      </c>
-      <c r="N11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get sostojanieupz =&gt; _sostojanieupz;</v>
-      </c>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="18" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="18" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="9"/>
@@ -1134,11 +896,11 @@
       <c r="A13" s="18"/>
       <c r="B13" s="5"/>
       <c r="C13" s="18" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="18" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="9"/>
@@ -1188,23 +950,11 @@
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialvklpolyar,</v>
-      </c>
-      <c r="N16" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialvklpolyar =&gt; _potencialvklpolyar;</v>
-      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="L16" s="6"/>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
@@ -1214,23 +964,11 @@
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialprot,</v>
-      </c>
-      <c r="N17" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialprot =&gt; _potencialprot;</v>
-      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="L17" s="6"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
@@ -1240,23 +978,11 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.edsupz,</v>
-      </c>
-      <c r="N18" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get edsupz =&gt; _edsupz;</v>
-      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="L18" s="6"/>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
@@ -1266,23 +992,11 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="15"/>
-      <c r="H19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.tokupz,</v>
-      </c>
-      <c r="N19" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get tokupz =&gt; _tokupz;</v>
-      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="L19" s="6"/>
+      <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1291,23 +1005,11 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.soprrast,</v>
-      </c>
-      <c r="N20" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get soprrast =&gt; _soprrast;</v>
-      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="L20" s="6"/>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
@@ -1316,23 +1018,9 @@
       <c r="E21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.udsoprgrunta,</v>
-      </c>
-      <c r="N21" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get udsoprgrunta =&gt; _udsoprgrunta;</v>
-      </c>
+      <c r="H21" s="16"/>
+      <c r="L21" s="6"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H22" s="17"/>
@@ -1340,137 +1028,39 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H23" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialvklsumm1,</v>
-      </c>
-      <c r="N23" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialvklsumm1 =&gt; _potencialvklsumm1;</v>
-      </c>
+      <c r="H23" s="16"/>
+      <c r="L23" s="6"/>
+      <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H24" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L24" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialvklpolyar1,</v>
-      </c>
-      <c r="N24" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialvklpolyar1 =&gt; _potencialvklpolyar1;</v>
-      </c>
+      <c r="H24" s="16"/>
+      <c r="L24" s="6"/>
+      <c r="N24" s="6"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H25" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J25" t="s">
-        <v>27</v>
-      </c>
-      <c r="L25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialprot1,</v>
-      </c>
-      <c r="N25" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialprot1 =&gt; _potencialprot1;</v>
-      </c>
+      <c r="H25" s="16"/>
+      <c r="L25" s="6"/>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H26" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.edsupz1,</v>
-      </c>
-      <c r="N26" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get edsupz1 =&gt; _edsupz1;</v>
-      </c>
+      <c r="H26" s="16"/>
+      <c r="L26" s="6"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.tokupz1,</v>
-      </c>
-      <c r="N27" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get tokupz1 =&gt; _tokupz1;</v>
-      </c>
+      <c r="H27" s="16"/>
+      <c r="L27" s="6"/>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H28" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.soprrast1,</v>
-      </c>
-      <c r="N28" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get soprrast1 =&gt; _soprrast1;</v>
-      </c>
+      <c r="H28" s="16"/>
+      <c r="L28" s="6"/>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H29" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" t="s">
-        <v>31</v>
-      </c>
-      <c r="L29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.udsoprgrunta1,</v>
-      </c>
-      <c r="N29" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get udsoprgrunta1 =&gt; _udsoprgrunta1;</v>
-      </c>
+      <c r="H29" s="16"/>
+      <c r="L29" s="6"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H30" s="17"/>
@@ -1478,137 +1068,39 @@
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H31" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" t="s">
-        <v>32</v>
-      </c>
-      <c r="L31" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialvklsumm2,</v>
-      </c>
-      <c r="N31" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialvklsumm2 =&gt; _potencialvklsumm2;</v>
-      </c>
+      <c r="H31" s="16"/>
+      <c r="L31" s="6"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H32" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" t="s">
-        <v>33</v>
-      </c>
-      <c r="L32" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialvklpolyar2,</v>
-      </c>
-      <c r="N32" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialvklpolyar2 =&gt; _potencialvklpolyar2;</v>
-      </c>
+      <c r="H32" s="16"/>
+      <c r="L32" s="6"/>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33" t="s">
-        <v>34</v>
-      </c>
-      <c r="L33" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.potencialprot2,</v>
-      </c>
-      <c r="N33" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get potencialprot2 =&gt; _potencialprot2;</v>
-      </c>
+      <c r="H33" s="16"/>
+      <c r="L33" s="6"/>
+      <c r="N33" s="6"/>
     </row>
     <row r="34" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H34" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" t="s">
-        <v>35</v>
-      </c>
-      <c r="L34" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.edsupz2,</v>
-      </c>
-      <c r="N34" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get edsupz2 =&gt; _edsupz2;</v>
-      </c>
+      <c r="H34" s="16"/>
+      <c r="L34" s="6"/>
+      <c r="N34" s="6"/>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H35" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" t="s">
-        <v>36</v>
-      </c>
-      <c r="L35" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.tokupz2,</v>
-      </c>
-      <c r="N35" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get tokupz2 =&gt; _tokupz2;</v>
-      </c>
+      <c r="H35" s="16"/>
+      <c r="L35" s="6"/>
+      <c r="N35" s="6"/>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I36" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" t="s">
-        <v>37</v>
-      </c>
-      <c r="L36" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.soprrast2,</v>
-      </c>
-      <c r="N36" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get soprrast2 =&gt; _soprrast2;</v>
-      </c>
+      <c r="H36" s="16"/>
+      <c r="L36" s="6"/>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H37" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I37" t="s">
-        <v>10</v>
-      </c>
-      <c r="J37" t="s">
-        <v>38</v>
-      </c>
-      <c r="L37" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>this.udsoprgrunta2,</v>
-      </c>
-      <c r="N37" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>String get udsoprgrunta2 =&gt; _udsoprgrunta2;</v>
-      </c>
+      <c r="H37" s="16"/>
+      <c r="L37" s="6"/>
+      <c r="N37" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>